<commit_message>
set private = auth
</commit_message>
<xml_diff>
--- a/night_guide.xlsx
+++ b/night_guide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="27540" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -331,6 +331,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -353,12 +354,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -694,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -766,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>

</xml_diff>